<commit_message>
Finishing CNPJ extraction to excel module
</commit_message>
<xml_diff>
--- a/CNPJ/CNPJ.xlsx
+++ b/CNPJ/CNPJ.xlsx
@@ -1,105 +1,55 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trjeh\PycharmProjects\AulasRPA\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91D68DC-B745-4419-BB54-A1F19CCA5D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-27120" yWindow="2880" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Dados" sheetId="1" r:id="rId1"/>
-    <sheet name="CNPJ" sheetId="2" r:id="rId2"/>
+    <sheet name="Dados" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="CNPJ" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>cnpj</t>
-  </si>
-  <si>
-    <t>nome</t>
-  </si>
-  <si>
-    <t>telefone</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>logradouro</t>
-  </si>
-  <si>
-    <t>bairro</t>
-  </si>
-  <si>
-    <t>municipio</t>
-  </si>
-  <si>
-    <t>uf</t>
-  </si>
-  <si>
-    <t>cep</t>
-  </si>
-  <si>
-    <t>atividade_principal</t>
-  </si>
-  <si>
-    <t>CNPJ</t>
-  </si>
-  <si>
-    <t>06947283000160</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="18"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -122,35 +72,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -438,57 +453,189 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="49.7109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
+    <row r="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>cnpj</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>nome</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>telefone</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="E1" s="5" t="inlineStr">
+        <is>
+          <t>logradouro</t>
+        </is>
+      </c>
+      <c r="F1" s="5" t="inlineStr">
+        <is>
+          <t>bairro</t>
+        </is>
+      </c>
+      <c r="G1" s="5" t="inlineStr">
+        <is>
+          <t>municipio</t>
+        </is>
+      </c>
+      <c r="H1" s="5" t="inlineStr">
+        <is>
+          <t>uf</t>
+        </is>
+      </c>
+      <c r="I1" s="5" t="inlineStr">
+        <is>
+          <t>cep</t>
+        </is>
+      </c>
+      <c r="J1" s="5" t="inlineStr">
+        <is>
+          <t>atividade_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33157312000162</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>IFOOD BENEFICIOS E SERVICOS LTDA.</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>AV DOS AUTONOMISTAS 1496</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>VILA YARA</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>OSASCO</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>06.020-902</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>[{'code': '82.99-7-02', 'text': 'Emissão de vales-alimentação, vales-transporte e similares'}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>06947283000160</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>GOOGLE INTERNATIONAL LLC</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1600 AMPHITHEATER PARKWAY</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>EXTERIOR</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>[{'code': '64.62-0-00', 'text': 'Holdings de instituições não-financeiras'}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>10573521000191</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MERCADO PAGO INSTITUICAO DE PAGAMENTO LTDA</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1 AV AVENIDA DAS NACOES UNIDAS, 3003</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>BONFIM</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>OSASCO</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>06.233-903</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>[{'code': '82.91-1-00', 'text': 'Atividades de cobranças e informações cadastrais'}]</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -497,46 +644,52 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.5703125" customWidth="1"/>
+    <col width="28.28515625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="3.5703125" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="23.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>CNPJ</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="23.65" customHeight="1">
+      <c r="A2" s="1" t="n">
         <v>33157312000162</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="23.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="23.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
+    <row r="3" ht="23.65" customHeight="1">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>06947283000160</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="23.65" customHeight="1">
+      <c r="A4" s="1" t="n">
         <v>10573521000191</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>55048956000155</v>
-      </c>
+    <row r="5">
+      <c r="A5" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="300" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>